<commit_message>
Update tambahan kolom pengisian, status, notelp, email, koordinat, sumber dan catatan
</commit_message>
<xml_diff>
--- a/Daftar Profiling SBR Kepala Madan.xlsx
+++ b/Daftar Profiling SBR Kepala Madan.xlsx
@@ -5,22 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuli\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kuliah\OtomatisasiSBR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD284493-93B3-4B39-AE67-65202404489F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1027943-5693-4E7F-A549-0BB66680E730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="203">
   <si>
     <t>IDSBR</t>
   </si>
@@ -611,13 +624,34 @@
   </si>
   <si>
     <t>Ada namun belum ada tanggapan dari pihak terkait</t>
+  </si>
+  <si>
+    <t>sdnegeribiloro@yahoo.com</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>sdnegerisukamaju17@gmail.com</t>
+  </si>
+  <si>
+    <t>Nomor Telepon</t>
+  </si>
+  <si>
+    <t>082239724951</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -626,6 +660,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -647,14 +693,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -726,16 +780,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5825167-6460-4617-B6A7-13F870BE837A}" name="Table1" displayName="Table1" ref="A1:G139" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G139" xr:uid="{C5825167-6460-4617-B6A7-13F870BE837A}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5825167-6460-4617-B6A7-13F870BE837A}" name="Table1" displayName="Table1" ref="A1:J139" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:J139" xr:uid="{C5825167-6460-4617-B6A7-13F870BE837A}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SD ALHILAAL (WALBELE)"/>
+        <filter val="SD ALHILAAL AIRTERNATE"/>
+        <filter val="SD ALHILAAL FOGI"/>
+        <filter val="SD ALHILAAL NANALI"/>
+        <filter val="SD ALHILAL FOGI"/>
+        <filter val="SD INPRES 01 DESA WAEKEKA"/>
+        <filter val="SD INPRES BALPETU"/>
+        <filter val="SD INPRES WAEHOTONG"/>
+        <filter val="SD INPRES WAEKEKA"/>
+        <filter val="SD NEGERI 02 KEPALA MADAN"/>
+        <filter val="SD NEGERI BATU LAYAR"/>
+        <filter val="SD NEGERI BILORO"/>
+        <filter val="SD NEGERI DARO SATAP"/>
+        <filter val="SD NEGERI SEKAT"/>
+        <filter val="SD NEGERI SUKA MAJU"/>
+        <filter val="SD NEGERI WAEHA"/>
+        <filter val="SD SWASTA 05 KEPALA MADAN"/>
+        <filter val="SDN AL HILAL AIR TERNATE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F197F7DA-FFB7-4622-AA08-CCC9EF20407F}" name="IDSBR"/>
     <tableColumn id="2" xr3:uid="{DF25E6B2-7F5B-408E-8D7A-AA7AAF73E801}" name="Nama"/>
     <tableColumn id="3" xr3:uid="{F24D0DB8-486E-4220-B747-D25B27233CB4}" name="Alamat"/>
     <tableColumn id="4" xr3:uid="{07DE8E23-5979-4A74-80C4-983D1386C66F}" name="Status"/>
+    <tableColumn id="11" xr3:uid="{5954E0D7-F963-4DD1-8A49-AE32DF4EADBB}" name="Nomor Telepon"/>
     <tableColumn id="5" xr3:uid="{32B14D7F-5062-4AAC-A654-994F90B003D1}" name="Email"/>
-    <tableColumn id="6" xr3:uid="{EE296787-F1FB-43DA-80E2-160B666947C4}" name="Sumber" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F5B091F5-95DD-41C3-A4F4-4F177CFF2392}" name="Catatan" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{381DC553-FB54-4935-BE0A-6B5D4234DE01}" name="Latitude"/>
+    <tableColumn id="9" xr3:uid="{3E2E6EA1-FE53-4120-B721-FA0CC7D7B624}" name="Longitude"/>
+    <tableColumn id="6" xr3:uid="{EE296787-F1FB-43DA-80E2-160B666947C4}" name="Sumber" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F5B091F5-95DD-41C3-A4F4-4F177CFF2392}" name="Catatan" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1028,20 +1108,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="1" max="4" width="14.36328125" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" customWidth="1"/>
+    <col min="7" max="8" width="14.36328125" style="5" customWidth="1"/>
+    <col min="9" max="10" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,17 +1136,26 @@
       <c r="D1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>97561073</v>
       </c>
@@ -1077,14 +1168,17 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>97561074</v>
       </c>
@@ -1097,14 +1191,17 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>97561076</v>
       </c>
@@ -1117,14 +1214,17 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>97561078</v>
       </c>
@@ -1137,14 +1237,17 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>97561079</v>
       </c>
@@ -1157,14 +1260,17 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>97561080</v>
       </c>
@@ -1177,14 +1283,17 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>97561081</v>
       </c>
@@ -1197,14 +1306,17 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>97561200</v>
       </c>
@@ -1217,14 +1329,17 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>97561180</v>
       </c>
@@ -1237,18 +1352,21 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>97561188</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
@@ -1257,14 +1375,23 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-3.1827000000000001</v>
+      </c>
+      <c r="H11" s="3">
+        <v>126.0172</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>97561189</v>
       </c>
@@ -1277,14 +1404,17 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>97561192</v>
       </c>
@@ -1297,18 +1427,21 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>97561207</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
@@ -1317,14 +1450,26 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" s="5">
+        <v>-3.3965999999999998</v>
+      </c>
+      <c r="H14" s="5">
+        <v>126.0774</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>97561206</v>
       </c>
@@ -1337,14 +1482,14 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>97561196</v>
       </c>
@@ -1357,14 +1502,17 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>97561195</v>
       </c>
@@ -1377,14 +1525,17 @@
       <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>97561205</v>
       </c>
@@ -1397,14 +1548,14 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>97561181</v>
       </c>
@@ -1417,14 +1568,17 @@
       <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>97561208</v>
       </c>
@@ -1437,14 +1591,14 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>97561415</v>
       </c>
@@ -1457,14 +1611,17 @@
       <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>97561416</v>
       </c>
@@ -1477,14 +1634,17 @@
       <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>97561417</v>
       </c>
@@ -1497,14 +1657,17 @@
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>97561412</v>
       </c>
@@ -1517,14 +1680,14 @@
       <c r="D24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>97561413</v>
       </c>
@@ -1537,14 +1700,17 @@
       <c r="D25" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>97561414</v>
       </c>
@@ -1557,14 +1723,14 @@
       <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I26" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>97561077</v>
       </c>
@@ -1577,14 +1743,17 @@
       <c r="D27" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>97561072</v>
       </c>
@@ -1597,14 +1766,17 @@
       <c r="D28" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>97561075</v>
       </c>
@@ -1617,14 +1789,17 @@
       <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>97561183</v>
       </c>
@@ -1637,14 +1812,17 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>97561184</v>
       </c>
@@ -1657,14 +1835,17 @@
       <c r="D31" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>97561185</v>
       </c>
@@ -1677,14 +1858,17 @@
       <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>97561182</v>
       </c>
@@ -1697,14 +1881,17 @@
       <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>97561202</v>
       </c>
@@ -1717,14 +1904,14 @@
       <c r="D34" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>97561203</v>
       </c>
@@ -1737,14 +1924,17 @@
       <c r="D35" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>97561193</v>
       </c>
@@ -1757,14 +1947,17 @@
       <c r="D36" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>97561199</v>
       </c>
@@ -1777,14 +1970,17 @@
       <c r="D37" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>97561201</v>
       </c>
@@ -1797,14 +1993,17 @@
       <c r="D38" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>97561204</v>
       </c>
@@ -1817,14 +2016,17 @@
       <c r="D39" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>97561194</v>
       </c>
@@ -1837,14 +2039,17 @@
       <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>97561190</v>
       </c>
@@ -1857,14 +2062,17 @@
       <c r="D41" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>97561191</v>
       </c>
@@ -1877,14 +2085,17 @@
       <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>97561198</v>
       </c>
@@ -1897,14 +2108,14 @@
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>97561179</v>
       </c>
@@ -1917,14 +2128,17 @@
       <c r="D44" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>97561197</v>
       </c>
@@ -1937,14 +2151,17 @@
       <c r="D45" t="s">
         <v>6</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>97561186</v>
       </c>
@@ -1957,14 +2174,17 @@
       <c r="D46" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>97561187</v>
       </c>
@@ -1977,14 +2197,17 @@
       <c r="D47" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2572599</v>
       </c>
@@ -1997,14 +2220,17 @@
       <c r="D48" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2594341</v>
       </c>
@@ -2017,14 +2243,17 @@
       <c r="D49" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2624661</v>
       </c>
@@ -2037,14 +2266,17 @@
       <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2665877</v>
       </c>
@@ -2057,14 +2289,14 @@
       <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2666250</v>
       </c>
@@ -2077,14 +2309,14 @@
       <c r="D52" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2674417</v>
       </c>
@@ -2097,14 +2329,17 @@
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2684182</v>
       </c>
@@ -2117,14 +2352,14 @@
       <c r="D54" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2708364</v>
       </c>
@@ -2137,14 +2372,14 @@
       <c r="D55" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I55" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2747329</v>
       </c>
@@ -2157,14 +2392,17 @@
       <c r="D56" t="s">
         <v>195</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G56" s="1" t="s">
+      <c r="E56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J56" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2834256</v>
       </c>
@@ -2177,14 +2415,17 @@
       <c r="D57" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2921198</v>
       </c>
@@ -2197,14 +2438,17 @@
       <c r="D58" t="s">
         <v>6</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>3029434</v>
       </c>
@@ -2217,14 +2461,17 @@
       <c r="D59" t="s">
         <v>190</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G59" s="1" t="s">
+      <c r="E59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>3090250</v>
       </c>
@@ -2237,14 +2484,17 @@
       <c r="D60" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3257130</v>
       </c>
@@ -2257,14 +2507,17 @@
       <c r="D61" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>3301535</v>
       </c>
@@ -2277,14 +2530,17 @@
       <c r="D62" t="s">
         <v>193</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>3304135</v>
       </c>
@@ -2297,14 +2553,17 @@
       <c r="D63" t="s">
         <v>102</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G63" s="1" t="s">
+      <c r="E63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>3348873</v>
       </c>
@@ -2317,14 +2576,17 @@
       <c r="D64" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>3427582</v>
       </c>
@@ -2337,14 +2599,17 @@
       <c r="D65" t="s">
         <v>190</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="E65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>3540340</v>
       </c>
@@ -2357,14 +2622,17 @@
       <c r="D66" t="s">
         <v>195</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="E66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>3563776</v>
       </c>
@@ -2377,14 +2645,14 @@
       <c r="D67" t="s">
         <v>6</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I67" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>3575301</v>
       </c>
@@ -2397,14 +2665,14 @@
       <c r="D68" t="s">
         <v>6</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>3595941</v>
       </c>
@@ -2417,14 +2685,17 @@
       <c r="D69" t="s">
         <v>195</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G69" s="1" t="s">
+      <c r="E69"/>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J69" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>3597967</v>
       </c>
@@ -2437,14 +2708,17 @@
       <c r="D70" t="s">
         <v>6</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>3605918</v>
       </c>
@@ -2457,14 +2731,17 @@
       <c r="D71" t="s">
         <v>6</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3623841</v>
       </c>
@@ -2477,14 +2754,17 @@
       <c r="D72" t="s">
         <v>6</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>3627918</v>
       </c>
@@ -2497,14 +2777,17 @@
       <c r="D73" t="s">
         <v>195</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G73" s="1" t="s">
+      <c r="E73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J73" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3628385</v>
       </c>
@@ -2517,14 +2800,17 @@
       <c r="D74" t="s">
         <v>6</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>3667235</v>
       </c>
@@ -2537,14 +2823,14 @@
       <c r="D75" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I75" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3670768</v>
       </c>
@@ -2557,14 +2843,17 @@
       <c r="D76" t="s">
         <v>102</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G76" s="1" t="s">
+      <c r="E76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J76" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3691831</v>
       </c>
@@ -2577,14 +2866,17 @@
       <c r="D77" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>3712937</v>
       </c>
@@ -2597,14 +2889,14 @@
       <c r="D78" t="s">
         <v>6</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I78" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>3715286</v>
       </c>
@@ -2617,14 +2909,17 @@
       <c r="D79" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3719130</v>
       </c>
@@ -2637,14 +2932,17 @@
       <c r="D80" t="s">
         <v>195</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G80" s="1" t="s">
+      <c r="E80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J80" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3722738</v>
       </c>
@@ -2657,14 +2955,17 @@
       <c r="D81" t="s">
         <v>195</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G81" s="1" t="s">
+      <c r="E81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J81" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>3726669</v>
       </c>
@@ -2677,14 +2978,17 @@
       <c r="D82" t="s">
         <v>6</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>3735726</v>
       </c>
@@ -2697,14 +3001,17 @@
       <c r="D83" t="s">
         <v>195</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G83" s="1" t="s">
+      <c r="E83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J83" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>3746672</v>
       </c>
@@ -2717,14 +3024,17 @@
       <c r="D84" t="s">
         <v>195</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G84" s="1" t="s">
+      <c r="E84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J84" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>3754240</v>
       </c>
@@ -2737,14 +3047,17 @@
       <c r="D85" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>3818977</v>
       </c>
@@ -2757,14 +3070,17 @@
       <c r="D86" t="s">
         <v>102</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G86" s="1" t="s">
+      <c r="E86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J86" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>3821657</v>
       </c>
@@ -2777,14 +3093,17 @@
       <c r="D87" t="s">
         <v>6</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3832940</v>
       </c>
@@ -2797,14 +3116,17 @@
       <c r="D88" t="s">
         <v>6</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>3839770</v>
       </c>
@@ -2817,14 +3139,17 @@
       <c r="D89" t="s">
         <v>190</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G89" s="1" t="s">
+      <c r="E89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J89" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>3862265</v>
       </c>
@@ -2837,14 +3162,17 @@
       <c r="D90" t="s">
         <v>195</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G90" s="1" t="s">
+      <c r="E90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J90" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>4141901</v>
       </c>
@@ -2857,14 +3185,17 @@
       <c r="D91" t="s">
         <v>6</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>4360507</v>
       </c>
@@ -2877,14 +3208,17 @@
       <c r="D92" t="s">
         <v>6</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>4407273</v>
       </c>
@@ -2897,14 +3231,17 @@
       <c r="D93" t="s">
         <v>6</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>4428482</v>
       </c>
@@ -2917,14 +3254,14 @@
       <c r="D94" t="s">
         <v>6</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I94" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>4433076</v>
       </c>
@@ -2937,14 +3274,14 @@
       <c r="D95" t="s">
         <v>6</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I95" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>4461202</v>
       </c>
@@ -2957,14 +3294,17 @@
       <c r="D96" t="s">
         <v>195</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G96" s="1" t="s">
+      <c r="E96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J96" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>4537317</v>
       </c>
@@ -2977,14 +3317,14 @@
       <c r="D97" t="s">
         <v>6</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I97" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>4554545</v>
       </c>
@@ -2997,14 +3337,17 @@
       <c r="D98" t="s">
         <v>102</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G98" s="1" t="s">
+      <c r="E98"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J98" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>4935662</v>
       </c>
@@ -3017,14 +3360,17 @@
       <c r="D99" t="s">
         <v>6</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E99"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>4935663</v>
       </c>
@@ -3037,14 +3383,17 @@
       <c r="D100" t="s">
         <v>6</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E100"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>4935664</v>
       </c>
@@ -3057,14 +3406,17 @@
       <c r="D101" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>4935665</v>
       </c>
@@ -3077,14 +3429,17 @@
       <c r="D102" t="s">
         <v>6</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>4935666</v>
       </c>
@@ -3097,14 +3452,17 @@
       <c r="D103" t="s">
         <v>6</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E103"/>
+      <c r="G103"/>
+      <c r="H103"/>
+      <c r="I103" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>4935667</v>
       </c>
@@ -3117,14 +3475,17 @@
       <c r="D104" t="s">
         <v>6</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E104"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>4935668</v>
       </c>
@@ -3137,14 +3498,17 @@
       <c r="D105" t="s">
         <v>6</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>4935669</v>
       </c>
@@ -3157,14 +3521,17 @@
       <c r="D106" t="s">
         <v>6</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E106"/>
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>4935670</v>
       </c>
@@ -3177,14 +3544,17 @@
       <c r="D107" t="s">
         <v>6</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E107"/>
+      <c r="G107"/>
+      <c r="H107"/>
+      <c r="I107" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>4935671</v>
       </c>
@@ -3197,14 +3567,17 @@
       <c r="D108" t="s">
         <v>6</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E108"/>
+      <c r="G108"/>
+      <c r="H108"/>
+      <c r="I108" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>4935672</v>
       </c>
@@ -3217,14 +3590,17 @@
       <c r="D109" t="s">
         <v>6</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E109"/>
+      <c r="G109"/>
+      <c r="H109"/>
+      <c r="I109" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>4935673</v>
       </c>
@@ -3237,14 +3613,17 @@
       <c r="D110" t="s">
         <v>6</v>
       </c>
-      <c r="F110" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E110"/>
+      <c r="G110"/>
+      <c r="H110"/>
+      <c r="I110" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>4935674</v>
       </c>
@@ -3257,14 +3636,17 @@
       <c r="D111" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E111"/>
+      <c r="G111"/>
+      <c r="H111"/>
+      <c r="I111" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>4935675</v>
       </c>
@@ -3277,14 +3659,17 @@
       <c r="D112" t="s">
         <v>6</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E112"/>
+      <c r="G112"/>
+      <c r="H112"/>
+      <c r="I112" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>4935676</v>
       </c>
@@ -3297,14 +3682,17 @@
       <c r="D113" t="s">
         <v>6</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E113"/>
+      <c r="G113"/>
+      <c r="H113"/>
+      <c r="I113" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>4935677</v>
       </c>
@@ -3317,14 +3705,17 @@
       <c r="D114" t="s">
         <v>6</v>
       </c>
-      <c r="F114" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E114"/>
+      <c r="G114"/>
+      <c r="H114"/>
+      <c r="I114" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>4935678</v>
       </c>
@@ -3337,14 +3728,17 @@
       <c r="D115" t="s">
         <v>6</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E115"/>
+      <c r="G115"/>
+      <c r="H115"/>
+      <c r="I115" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>4935679</v>
       </c>
@@ -3357,14 +3751,17 @@
       <c r="D116" t="s">
         <v>6</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E116"/>
+      <c r="G116"/>
+      <c r="H116"/>
+      <c r="I116" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>4935680</v>
       </c>
@@ -3377,14 +3774,17 @@
       <c r="D117" t="s">
         <v>6</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E117"/>
+      <c r="G117"/>
+      <c r="H117"/>
+      <c r="I117" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>4935681</v>
       </c>
@@ -3397,14 +3797,17 @@
       <c r="D118" t="s">
         <v>6</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E118"/>
+      <c r="G118"/>
+      <c r="H118"/>
+      <c r="I118" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>4935682</v>
       </c>
@@ -3417,14 +3820,17 @@
       <c r="D119" t="s">
         <v>6</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E119"/>
+      <c r="G119"/>
+      <c r="H119"/>
+      <c r="I119" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>4935683</v>
       </c>
@@ -3437,14 +3843,17 @@
       <c r="D120" t="s">
         <v>6</v>
       </c>
-      <c r="F120" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E120"/>
+      <c r="G120"/>
+      <c r="H120"/>
+      <c r="I120" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>4935684</v>
       </c>
@@ -3457,14 +3866,17 @@
       <c r="D121" t="s">
         <v>6</v>
       </c>
-      <c r="F121" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E121"/>
+      <c r="G121"/>
+      <c r="H121"/>
+      <c r="I121" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>4935685</v>
       </c>
@@ -3477,14 +3889,17 @@
       <c r="D122" t="s">
         <v>6</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E122"/>
+      <c r="G122"/>
+      <c r="H122"/>
+      <c r="I122" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>4936418</v>
       </c>
@@ -3497,14 +3912,17 @@
       <c r="D123" t="s">
         <v>6</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E123"/>
+      <c r="G123"/>
+      <c r="H123"/>
+      <c r="I123" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>4977600</v>
       </c>
@@ -3517,14 +3935,17 @@
       <c r="D124" t="s">
         <v>6</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E124"/>
+      <c r="G124"/>
+      <c r="H124"/>
+      <c r="I124" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>5426044</v>
       </c>
@@ -3537,14 +3958,17 @@
       <c r="D125" t="s">
         <v>6</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E125"/>
+      <c r="G125"/>
+      <c r="H125"/>
+      <c r="I125" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>5426045</v>
       </c>
@@ -3557,14 +3981,17 @@
       <c r="D126" t="s">
         <v>6</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E126"/>
+      <c r="G126"/>
+      <c r="H126"/>
+      <c r="I126" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>5426046</v>
       </c>
@@ -3577,14 +4004,17 @@
       <c r="D127" t="s">
         <v>6</v>
       </c>
-      <c r="F127" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E127"/>
+      <c r="G127"/>
+      <c r="H127"/>
+      <c r="I127" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>5426047</v>
       </c>
@@ -3597,14 +4027,17 @@
       <c r="D128" t="s">
         <v>6</v>
       </c>
-      <c r="F128" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E128"/>
+      <c r="G128"/>
+      <c r="H128"/>
+      <c r="I128" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>5426048</v>
       </c>
@@ -3617,14 +4050,17 @@
       <c r="D129" t="s">
         <v>6</v>
       </c>
-      <c r="F129" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E129"/>
+      <c r="G129"/>
+      <c r="H129"/>
+      <c r="I129" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>5426049</v>
       </c>
@@ -3637,14 +4073,17 @@
       <c r="D130" t="s">
         <v>6</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E130"/>
+      <c r="G130"/>
+      <c r="H130"/>
+      <c r="I130" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>5426050</v>
       </c>
@@ -3657,14 +4096,17 @@
       <c r="D131" t="s">
         <v>6</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E131"/>
+      <c r="G131"/>
+      <c r="H131"/>
+      <c r="I131" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>5427050</v>
       </c>
@@ -3677,14 +4119,17 @@
       <c r="D132" t="s">
         <v>6</v>
       </c>
-      <c r="F132" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E132"/>
+      <c r="G132"/>
+      <c r="H132"/>
+      <c r="I132" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>5427051</v>
       </c>
@@ -3697,14 +4142,17 @@
       <c r="D133" t="s">
         <v>6</v>
       </c>
-      <c r="F133" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E133"/>
+      <c r="G133"/>
+      <c r="H133"/>
+      <c r="I133" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>5427052</v>
       </c>
@@ -3717,14 +4165,17 @@
       <c r="D134" t="s">
         <v>6</v>
       </c>
-      <c r="F134" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E134"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>5427053</v>
       </c>
@@ -3737,14 +4188,17 @@
       <c r="D135" t="s">
         <v>6</v>
       </c>
-      <c r="F135" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E135"/>
+      <c r="G135"/>
+      <c r="H135"/>
+      <c r="I135" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>5781161</v>
       </c>
@@ -3757,14 +4211,17 @@
       <c r="D136" t="s">
         <v>6</v>
       </c>
-      <c r="F136" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E136"/>
+      <c r="G136"/>
+      <c r="H136"/>
+      <c r="I136" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>5781300</v>
       </c>
@@ -3777,14 +4234,17 @@
       <c r="D137" t="s">
         <v>6</v>
       </c>
-      <c r="F137" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E137"/>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="I137" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>5962820</v>
       </c>
@@ -3797,14 +4257,17 @@
       <c r="D138" t="s">
         <v>6</v>
       </c>
-      <c r="F138" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E138"/>
+      <c r="G138"/>
+      <c r="H138"/>
+      <c r="I138" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>5963435</v>
       </c>
@@ -3817,17 +4280,25 @@
       <c r="D139" t="s">
         <v>6</v>
       </c>
-      <c r="F139" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G139" s="1" t="s">
+      <c r="E139"/>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J139" s="1" t="s">
         <v>192</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{91ABD16C-596F-4276-99FE-49ED9D7C8BFA}"/>
+    <hyperlink ref="F14" r:id="rId2" xr:uid="{26E1FEAC-E651-4FE8-9E72-D09CFFCF59E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>